<commit_message>
AutoCommit_11 апреля 2024 г. 15:34:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\2ОИБАС1022\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Sibirev I. V." sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>2ОИБАС1022: Операционные системы (Сибирев И. В.) - I семестр</t>
   </si>
@@ -139,10 +144,7 @@
     <t>Инд9</t>
   </si>
   <si>
-    <t>симма</t>
-  </si>
-  <si>
-    <t>ТкЗима</t>
+    <t>Лаб6</t>
   </si>
 </sst>
 </file>
@@ -162,7 +164,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,8 +183,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -214,11 +222,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -242,6 +261,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -548,29 +570,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U17" sqref="U17:V17"/>
+      <selection pane="bottomRight" activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="13" width="5.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="4" max="13" width="5.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="29.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="29.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -616,14 +638,14 @@
       <c r="Q2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="R2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+    </row>
+    <row r="3" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>IF(B3=C3,A2+1,"---")</f>
         <v>1</v>
@@ -641,15 +663,8 @@
         <v>4</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="S3">
-        <f>SUM(D3:Q3)</f>
-        <v>9</v>
-      </c>
-      <c r="T3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A28" si="0">IF(B4=C4,A3+1,"---")</f>
         <v>2</v>
@@ -666,15 +681,9 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="S4" s="9">
-        <f t="shared" ref="S4:S37" si="1">SUM(D4:Q4)</f>
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -707,15 +716,12 @@
         <v>5</v>
       </c>
       <c r="Q5" s="2"/>
-      <c r="S5" s="9">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="T5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="11">
+        <v>5</v>
+      </c>
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -732,15 +738,9 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-      <c r="S6" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -779,15 +779,9 @@
         <v>5</v>
       </c>
       <c r="Q7" s="2"/>
-      <c r="S7" s="9">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="T7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -808,15 +802,9 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-      <c r="S8" s="9">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="T8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -845,15 +833,9 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-      <c r="S9" s="9">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="T9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -870,15 +852,9 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
-      <c r="S10" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -907,15 +883,9 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
-      <c r="S11" s="9">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="T11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -932,15 +902,9 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-      <c r="S12" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -969,15 +933,9 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="S13" s="9">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="T13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S13" s="9"/>
+    </row>
+    <row r="14" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -994,15 +952,9 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
-      <c r="S14" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S14" s="9"/>
+    </row>
+    <row r="15" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1019,15 +971,9 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
-      <c r="S15" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S15" s="9"/>
+    </row>
+    <row r="16" spans="1:21" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1046,15 +992,9 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-      <c r="S16" s="9">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="T16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S16" s="9"/>
+    </row>
+    <row r="17" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1090,15 +1030,12 @@
         <v>5</v>
       </c>
       <c r="Q17" s="2"/>
-      <c r="S17" s="9">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="T17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R17" s="11">
+        <v>5</v>
+      </c>
+      <c r="S17" s="9"/>
+    </row>
+    <row r="18" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1119,15 +1056,9 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
-      <c r="S18" s="9">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="T18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S18" s="9"/>
+    </row>
+    <row r="19" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1144,15 +1075,9 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="S19" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S19" s="9"/>
+    </row>
+    <row r="20" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1180,15 +1105,9 @@
       <c r="Q20" s="3">
         <v>4</v>
       </c>
-      <c r="S20" s="9">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="T20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S20" s="9"/>
+    </row>
+    <row r="21" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1207,15 +1126,9 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="S21" s="9">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="T21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S21" s="9"/>
+    </row>
+    <row r="22" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1236,15 +1149,9 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="S22" s="9">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="T22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S22" s="9"/>
+    </row>
+    <row r="23" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1274,15 +1181,9 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
-      <c r="S23" s="9">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="T23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S23" s="9"/>
+    </row>
+    <row r="24" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1309,15 +1210,9 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
-      <c r="S24" s="9">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="T24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S24" s="9"/>
+    </row>
+    <row r="25" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1334,15 +1229,9 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-      <c r="S25" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S25" s="9"/>
+    </row>
+    <row r="26" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1359,15 +1248,9 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="S26" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S26" s="9"/>
+    </row>
+    <row r="27" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1393,15 +1276,12 @@
       <c r="Q27" s="3">
         <v>4</v>
       </c>
-      <c r="S27" s="9">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="T27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>5</v>
+      </c>
+      <c r="S27" s="9"/>
+    </row>
+    <row r="28" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1425,15 +1305,9 @@
       <c r="Q28" s="3">
         <v>4</v>
       </c>
-      <c r="S28" s="9">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="T28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S28" s="9"/>
+    </row>
+    <row r="29" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1455,12 +1329,9 @@
       <c r="Q29" s="3">
         <v>4</v>
       </c>
-      <c r="S29" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S29" s="9"/>
+    </row>
+    <row r="30" spans="1:19" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1482,12 +1353,9 @@
       <c r="Q30" s="3">
         <v>4</v>
       </c>
-      <c r="S30" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S30" s="9"/>
+    </row>
+    <row r="31" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1509,12 +1377,9 @@
       <c r="Q31" s="3">
         <v>4</v>
       </c>
-      <c r="S31" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S31" s="9"/>
+    </row>
+    <row r="32" spans="1:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
@@ -1536,12 +1401,9 @@
       <c r="Q32" s="3">
         <v>4</v>
       </c>
-      <c r="S32" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="3:19" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S32" s="9"/>
+    </row>
+    <row r="33" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
         <v>25</v>
       </c>
@@ -1563,12 +1425,9 @@
       <c r="Q33" s="3">
         <v>4</v>
       </c>
-      <c r="S33" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="3:19" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S33" s="9"/>
+    </row>
+    <row r="34" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>25</v>
       </c>
@@ -1590,12 +1449,9 @@
       <c r="Q34" s="3">
         <v>4</v>
       </c>
-      <c r="S34" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="3:19" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S34" s="9"/>
+    </row>
+    <row r="35" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
         <v>25</v>
       </c>
@@ -1617,12 +1473,9 @@
       <c r="Q35" s="3">
         <v>4</v>
       </c>
-      <c r="S35" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="3:19" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S35" s="9"/>
+    </row>
+    <row r="36" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
         <v>25</v>
       </c>
@@ -1644,12 +1497,9 @@
       <c r="Q36" s="3">
         <v>4</v>
       </c>
-      <c r="S36" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="3:19" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S36" s="9"/>
+    </row>
+    <row r="37" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
         <v>25</v>
       </c>
@@ -1671,12 +1521,9 @@
       <c r="Q37" s="3">
         <v>4</v>
       </c>
-      <c r="S37" s="9">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="3:19" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="S37" s="9"/>
+    </row>
+    <row r="38" spans="3:19" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="S3:S37">

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 9:19:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t>Ашурова Шахруза</t>
   </si>
@@ -163,6 +163,21 @@
   </si>
   <si>
     <t>Л 6</t>
+  </si>
+  <si>
+    <t>Л 7</t>
+  </si>
+  <si>
+    <t>Л 8</t>
+  </si>
+  <si>
+    <t>Л 9</t>
+  </si>
+  <si>
+    <t>Л 10</t>
+  </si>
+  <si>
+    <t>Л 11</t>
   </si>
 </sst>
 </file>
@@ -588,13 +603,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:AD37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -603,10 +618,11 @@
     <col min="2" max="2" width="18.81640625" customWidth="1"/>
     <col min="3" max="3" width="21.54296875" customWidth="1"/>
     <col min="4" max="12" width="3.1796875" customWidth="1"/>
-    <col min="13" max="21" width="3.26953125" customWidth="1"/>
+    <col min="13" max="20" width="3.26953125" customWidth="1"/>
+    <col min="21" max="26" width="3.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="29.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="29.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
@@ -664,15 +680,29 @@
       <c r="U1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10" t="s">
+      <c r="V1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="AB1" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>IF(B2=C2,A1+1,"---")</f>
         <v>1</v>
@@ -690,14 +720,17 @@
         <v>4</v>
       </c>
       <c r="T2" s="1"/>
-      <c r="W2">
+      <c r="Z2">
+        <v>5</v>
+      </c>
+      <c r="AA2">
         <v>10</v>
       </c>
-      <c r="X2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f t="shared" ref="A3:A27" si="0">IF(B3=C3,A2+1,"---")</f>
         <v>2</v>
@@ -715,17 +748,20 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="V3" s="9"/>
-      <c r="W3">
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
         <v>25</v>
       </c>
-      <c r="X3">
-        <v>4</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="AB3">
+        <v>4</v>
+      </c>
+      <c r="AC3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -783,14 +819,14 @@
         <v>5</v>
       </c>
       <c r="V4" s="9"/>
-      <c r="W4">
+      <c r="AA4">
         <v>3</v>
       </c>
-      <c r="X4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -808,14 +844,14 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="V5" s="9"/>
-      <c r="W5">
+      <c r="AA5">
         <v>28</v>
       </c>
-      <c r="X5">
+      <c r="AB5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -855,14 +891,14 @@
       </c>
       <c r="T6" s="2"/>
       <c r="V6" s="9"/>
-      <c r="W6">
+      <c r="AA6">
         <v>26</v>
       </c>
-      <c r="X6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -884,14 +920,17 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="V7" s="9"/>
-      <c r="W7">
+      <c r="Z7">
+        <v>5</v>
+      </c>
+      <c r="AA7">
         <v>18</v>
       </c>
-      <c r="X7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -939,14 +978,14 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="V8" s="9"/>
-      <c r="W8">
+      <c r="AA8">
         <v>21</v>
       </c>
-      <c r="X8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -964,14 +1003,14 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="V9" s="9"/>
-      <c r="W9">
+      <c r="AA9">
         <v>11</v>
       </c>
-      <c r="X9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1016,14 +1055,14 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="V10" s="9"/>
-      <c r="W10">
+      <c r="AA10">
         <v>22</v>
       </c>
-      <c r="X10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1041,14 +1080,14 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="V11" s="9"/>
-      <c r="W11">
+      <c r="AA11">
         <v>9</v>
       </c>
-      <c r="X11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1078,14 +1117,14 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="V12" s="9"/>
-      <c r="W12">
+      <c r="AA12">
         <v>2</v>
       </c>
-      <c r="X12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1103,14 +1142,14 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="V13" s="9"/>
-      <c r="W13">
+      <c r="AA13">
         <v>23</v>
       </c>
-      <c r="X13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1143,20 +1182,20 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="V14" s="9"/>
-      <c r="W14">
+      <c r="AA14">
         <v>24</v>
       </c>
-      <c r="X14">
-        <v>5</v>
-      </c>
-      <c r="Y14">
+      <c r="AB14">
+        <v>5</v>
+      </c>
+      <c r="AC14">
         <v>10</v>
       </c>
-      <c r="Z14">
+      <c r="AD14">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1176,17 +1215,17 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="V15" s="9"/>
-      <c r="W15">
+      <c r="AA15">
         <v>25</v>
       </c>
-      <c r="X15">
-        <v>4</v>
-      </c>
-      <c r="Z15" t="s">
+      <c r="AB15">
+        <v>4</v>
+      </c>
+      <c r="AD15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1226,14 +1265,14 @@
         <v>5</v>
       </c>
       <c r="V16" s="9"/>
-      <c r="W16">
+      <c r="AA16">
         <v>1</v>
       </c>
-      <c r="X16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1255,14 +1294,14 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="V17" s="9"/>
-      <c r="W17">
+      <c r="AA17">
         <v>3</v>
       </c>
-      <c r="X17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1280,14 +1319,14 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="V18" s="9"/>
-      <c r="W18">
+      <c r="AA18">
         <v>11</v>
       </c>
-      <c r="X18">
+      <c r="AB18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1334,14 +1373,14 @@
         <v>4</v>
       </c>
       <c r="V19" s="9"/>
-      <c r="W19">
+      <c r="AA19">
         <v>25</v>
       </c>
-      <c r="X19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1361,14 +1400,17 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="V20" s="9"/>
-      <c r="W20">
+      <c r="Z20">
+        <v>5</v>
+      </c>
+      <c r="AA20">
         <v>10</v>
       </c>
-      <c r="X20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1390,14 +1432,14 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="V21" s="9"/>
-      <c r="W21">
+      <c r="AA21">
         <v>9</v>
       </c>
-      <c r="X21">
+      <c r="AB21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1428,17 +1470,20 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="V22" s="9"/>
-      <c r="W22">
+      <c r="Z22">
+        <v>5</v>
+      </c>
+      <c r="AA22">
         <v>16</v>
       </c>
-      <c r="X22">
+      <c r="AB22">
         <v>3</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AD22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1481,14 +1526,14 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="V23" s="9"/>
-      <c r="W23">
+      <c r="AA23">
         <v>6</v>
       </c>
-      <c r="X23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1506,14 +1551,14 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="V24" s="9"/>
-      <c r="W24">
+      <c r="AA24">
         <v>24</v>
       </c>
-      <c r="X24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1531,14 +1576,14 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="V25" s="9"/>
-      <c r="W25">
+      <c r="AA25">
         <v>8</v>
       </c>
-      <c r="X25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1568,14 +1613,14 @@
         <v>5</v>
       </c>
       <c r="V26" s="9"/>
-      <c r="W26">
+      <c r="AA26">
         <v>12</v>
       </c>
-      <c r="X26">
+      <c r="AB26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1600,14 +1645,14 @@
         <v>4</v>
       </c>
       <c r="V27" s="9"/>
-      <c r="W27">
+      <c r="AA27">
         <v>6</v>
       </c>
-      <c r="X27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
       <c r="D28" s="3"/>
       <c r="E28" s="9"/>
@@ -1625,7 +1670,7 @@
       <c r="T28" s="3"/>
       <c r="V28" s="9"/>
     </row>
-    <row r="29" spans="1:26" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" ht="14.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="3"/>
       <c r="E29" s="9"/>
@@ -1643,7 +1688,7 @@
       <c r="T29" s="3"/>
       <c r="V29" s="9"/>
     </row>
-    <row r="30" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
       <c r="D30" s="3"/>
       <c r="E30" s="9"/>
@@ -1661,7 +1706,7 @@
       <c r="T30" s="3"/>
       <c r="V30" s="9"/>
     </row>
-    <row r="31" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="3"/>
       <c r="E31" s="9"/>
@@ -1679,7 +1724,7 @@
       <c r="T31" s="3"/>
       <c r="V31" s="9"/>
     </row>
-    <row r="32" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="3"/>
       <c r="E32" s="9"/>
@@ -1784,7 +1829,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X27">
+  <conditionalFormatting sqref="AB2:AB27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 9:29:26_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -609,7 +609,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Z3" sqref="Z3"/>
+      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -720,6 +720,15 @@
         <v>4</v>
       </c>
       <c r="T2" s="1"/>
+      <c r="W2">
+        <v>5</v>
+      </c>
+      <c r="X2">
+        <v>5</v>
+      </c>
+      <c r="Y2">
+        <v>5</v>
+      </c>
       <c r="Z2">
         <v>5</v>
       </c>
@@ -748,6 +757,15 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="V3" s="9"/>
+      <c r="W3">
+        <v>5</v>
+      </c>
+      <c r="X3">
+        <v>5</v>
+      </c>
+      <c r="Y3">
+        <v>5</v>
+      </c>
       <c r="Z3">
         <v>5</v>
       </c>
@@ -920,6 +938,15 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="V7" s="9"/>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7">
+        <v>5</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
       <c r="Z7">
         <v>5</v>
       </c>
@@ -1399,7 +1426,18 @@
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
-      <c r="V20" s="9"/>
+      <c r="V20" s="9">
+        <v>5</v>
+      </c>
+      <c r="W20">
+        <v>5</v>
+      </c>
+      <c r="X20">
+        <v>5</v>
+      </c>
+      <c r="Y20">
+        <v>5</v>
+      </c>
       <c r="Z20">
         <v>5</v>
       </c>
@@ -1469,7 +1507,18 @@
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
-      <c r="V22" s="9"/>
+      <c r="V22" s="9">
+        <v>5</v>
+      </c>
+      <c r="W22">
+        <v>5</v>
+      </c>
+      <c r="X22">
+        <v>5</v>
+      </c>
+      <c r="Y22">
+        <v>5</v>
+      </c>
       <c r="Z22">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 9:31:14_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -609,7 +609,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V21" sqref="V21"/>
+      <selection pane="bottomRight" activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1320,7 +1320,9 @@
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
-      <c r="V17" s="9"/>
+      <c r="V17" s="9">
+        <v>5</v>
+      </c>
       <c r="AA17">
         <v>3</v>
       </c>
@@ -1399,7 +1401,9 @@
       <c r="T19" s="3">
         <v>4</v>
       </c>
-      <c r="V19" s="9"/>
+      <c r="V19" s="9">
+        <v>5</v>
+      </c>
       <c r="AA19">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 9:36:02_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -297,6 +297,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -609,7 +612,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V18" sqref="V18"/>
+      <selection pane="bottomRight" activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -720,6 +723,9 @@
         <v>4</v>
       </c>
       <c r="T2" s="1"/>
+      <c r="V2">
+        <v>5</v>
+      </c>
       <c r="W2">
         <v>5</v>
       </c>
@@ -756,7 +762,9 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
-      <c r="V3" s="9"/>
+      <c r="V3" s="9">
+        <v>5</v>
+      </c>
       <c r="W3">
         <v>5</v>
       </c>
@@ -836,7 +844,9 @@
       <c r="U4" s="11">
         <v>5</v>
       </c>
-      <c r="V4" s="9"/>
+      <c r="V4" s="12">
+        <v>5</v>
+      </c>
       <c r="AA4">
         <v>3</v>
       </c>
@@ -937,7 +947,9 @@
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
-      <c r="V7" s="9"/>
+      <c r="V7" s="9">
+        <v>5</v>
+      </c>
       <c r="W7">
         <v>5</v>
       </c>
@@ -1081,7 +1093,9 @@
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
-      <c r="V10" s="9"/>
+      <c r="V10" s="9">
+        <v>5</v>
+      </c>
       <c r="AA10">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 9:51:37_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -612,7 +612,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V2" sqref="V2"/>
+      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -722,7 +722,18 @@
       <c r="G2" s="4">
         <v>4</v>
       </c>
-      <c r="T2" s="1"/>
+      <c r="R2">
+        <v>5</v>
+      </c>
+      <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2" s="1">
+        <v>5</v>
+      </c>
+      <c r="U2">
+        <v>5</v>
+      </c>
       <c r="V2">
         <v>5</v>
       </c>
@@ -759,9 +770,18 @@
       <c r="D3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
+      <c r="R3" s="2">
+        <v>5</v>
+      </c>
+      <c r="S3" s="2">
+        <v>5</v>
+      </c>
+      <c r="T3" s="2">
+        <v>5</v>
+      </c>
+      <c r="U3">
+        <v>5</v>
+      </c>
       <c r="V3" s="9">
         <v>5</v>
       </c>
@@ -944,9 +964,18 @@
         <v>5</v>
       </c>
       <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
+      <c r="R7" s="2">
+        <v>5</v>
+      </c>
+      <c r="S7" s="2">
+        <v>5</v>
+      </c>
+      <c r="T7" s="2">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>5</v>
+      </c>
       <c r="V7" s="9">
         <v>5</v>
       </c>
@@ -1016,6 +1045,9 @@
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
+      <c r="U8">
+        <v>5</v>
+      </c>
       <c r="V8" s="9"/>
       <c r="AA8">
         <v>21</v>
@@ -1093,6 +1125,9 @@
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
+      <c r="U10">
+        <v>5</v>
+      </c>
       <c r="V10" s="9">
         <v>5</v>
       </c>
@@ -1333,7 +1368,12 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
+      <c r="T17" s="2">
+        <v>5</v>
+      </c>
+      <c r="U17">
+        <v>5</v>
+      </c>
       <c r="V17" s="9">
         <v>5</v>
       </c>
@@ -1415,6 +1455,9 @@
       <c r="T19" s="3">
         <v>4</v>
       </c>
+      <c r="U19" s="12">
+        <v>5</v>
+      </c>
       <c r="V19" s="9">
         <v>5</v>
       </c>
@@ -1441,9 +1484,18 @@
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
+      <c r="R20" s="2">
+        <v>5</v>
+      </c>
+      <c r="S20" s="2">
+        <v>5</v>
+      </c>
+      <c r="T20" s="2">
+        <v>5</v>
+      </c>
+      <c r="U20">
+        <v>5</v>
+      </c>
       <c r="V20" s="9">
         <v>5</v>
       </c>
@@ -1522,9 +1574,18 @@
       <c r="Q22" s="3">
         <v>5</v>
       </c>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
+      <c r="R22" s="2">
+        <v>5</v>
+      </c>
+      <c r="S22" s="2">
+        <v>5</v>
+      </c>
+      <c r="T22" s="2">
+        <v>5</v>
+      </c>
+      <c r="U22">
+        <v>5</v>
+      </c>
       <c r="V22" s="9">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 9:57:02_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -612,7 +612,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -722,6 +722,9 @@
       <c r="G2" s="4">
         <v>4</v>
       </c>
+      <c r="Q2">
+        <v>5</v>
+      </c>
       <c r="R2">
         <v>5</v>
       </c>
@@ -819,6 +822,9 @@
         <v>1</v>
       </c>
       <c r="D4" s="5">
+        <v>5</v>
+      </c>
+      <c r="F4">
         <v>5</v>
       </c>
       <c r="G4" s="6">
@@ -963,7 +969,9 @@
       <c r="P7" s="3">
         <v>5</v>
       </c>
-      <c r="Q7" s="2"/>
+      <c r="Q7" s="2">
+        <v>5</v>
+      </c>
       <c r="R7" s="2">
         <v>5</v>
       </c>
@@ -1016,6 +1024,9 @@
         <v>5</v>
       </c>
       <c r="G8" s="4">
+        <v>5</v>
+      </c>
+      <c r="I8">
         <v>5</v>
       </c>
       <c r="J8">
@@ -1116,6 +1127,9 @@
       <c r="N10">
         <v>5</v>
       </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
       <c r="P10" s="3">
         <v>5</v>
       </c>
@@ -1249,7 +1263,13 @@
       <c r="L14">
         <v>5</v>
       </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
       <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14">
         <v>5</v>
       </c>
       <c r="P14" s="2"/>
@@ -1365,7 +1385,9 @@
       <c r="P17" s="3">
         <v>5</v>
       </c>
-      <c r="Q17" s="2"/>
+      <c r="Q17" s="2">
+        <v>5</v>
+      </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2">
@@ -1483,7 +1505,9 @@
         <v>5</v>
       </c>
       <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
+      <c r="Q20" s="2">
+        <v>5</v>
+      </c>
       <c r="R20" s="2">
         <v>5</v>
       </c>
@@ -1623,6 +1647,9 @@
         <v>20</v>
       </c>
       <c r="D23" s="2"/>
+      <c r="F23">
+        <v>5</v>
+      </c>
       <c r="G23" s="4">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 13:17:19_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -300,6 +300,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -612,7 +615,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -873,6 +876,15 @@
       <c r="V4" s="12">
         <v>5</v>
       </c>
+      <c r="W4" s="12">
+        <v>5</v>
+      </c>
+      <c r="X4">
+        <v>5</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
       <c r="AA4">
         <v>3</v>
       </c>
@@ -1060,6 +1072,18 @@
         <v>5</v>
       </c>
       <c r="V8" s="9"/>
+      <c r="W8">
+        <v>5</v>
+      </c>
+      <c r="X8">
+        <v>5</v>
+      </c>
+      <c r="Y8">
+        <v>5</v>
+      </c>
+      <c r="Z8">
+        <v>5</v>
+      </c>
       <c r="AA8">
         <v>21</v>
       </c>
@@ -1145,6 +1169,12 @@
       <c r="V10" s="9">
         <v>5</v>
       </c>
+      <c r="W10">
+        <v>5</v>
+      </c>
+      <c r="Y10">
+        <v>5</v>
+      </c>
       <c r="AA10">
         <v>22</v>
       </c>
@@ -1303,14 +1333,40 @@
         <v>12</v>
       </c>
       <c r="D15" s="2"/>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
       <c r="P15" s="3">
         <v>5</v>
       </c>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
+      <c r="Q15" s="2">
+        <v>5</v>
+      </c>
+      <c r="R15" s="2">
+        <v>5</v>
+      </c>
+      <c r="S15" s="2">
+        <v>5</v>
+      </c>
+      <c r="T15" s="2">
+        <v>5</v>
+      </c>
+      <c r="U15">
+        <v>5</v>
+      </c>
       <c r="V15" s="9"/>
+      <c r="W15">
+        <v>5</v>
+      </c>
+      <c r="Y15">
+        <v>5</v>
+      </c>
+      <c r="Z15">
+        <v>5</v>
+      </c>
       <c r="AA15">
         <v>25</v>
       </c>
@@ -1397,6 +1453,12 @@
         <v>5</v>
       </c>
       <c r="V17" s="9">
+        <v>5</v>
+      </c>
+      <c r="W17" s="13">
+        <v>5</v>
+      </c>
+      <c r="X17">
         <v>5</v>
       </c>
       <c r="AA17">
@@ -1481,6 +1543,12 @@
         <v>5</v>
       </c>
       <c r="V19" s="9">
+        <v>5</v>
+      </c>
+      <c r="W19">
+        <v>5</v>
+      </c>
+      <c r="X19">
         <v>5</v>
       </c>
       <c r="AA19">
@@ -1972,7 +2040,7 @@
     <row r="37" spans="3:22" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="V2:V36">
+  <conditionalFormatting sqref="V2:V36 W4">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 21:12:55_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -615,7 +615,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -882,6 +882,9 @@
       <c r="X4">
         <v>5</v>
       </c>
+      <c r="Y4">
+        <v>5</v>
+      </c>
       <c r="Z4">
         <v>5</v>
       </c>
@@ -1172,6 +1175,9 @@
       <c r="W10">
         <v>5</v>
       </c>
+      <c r="X10">
+        <v>5</v>
+      </c>
       <c r="Y10">
         <v>5</v>
       </c>
@@ -1237,6 +1243,15 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="V12" s="9"/>
+      <c r="W12">
+        <v>5</v>
+      </c>
+      <c r="X12">
+        <v>5</v>
+      </c>
+      <c r="Y12">
+        <v>5</v>
+      </c>
       <c r="AA12">
         <v>2</v>
       </c>
@@ -1308,6 +1323,9 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="V14" s="9"/>
+      <c r="W14">
+        <v>5</v>
+      </c>
       <c r="AA14">
         <v>24</v>
       </c>
@@ -1359,6 +1377,9 @@
       </c>
       <c r="V15" s="9"/>
       <c r="W15">
+        <v>5</v>
+      </c>
+      <c r="X15">
         <v>5</v>
       </c>
       <c r="Y15">
@@ -1749,6 +1770,12 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="V23" s="9"/>
+      <c r="W23">
+        <v>5</v>
+      </c>
+      <c r="X23">
+        <v>5</v>
+      </c>
       <c r="AA23">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 21:16:09_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -270,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -303,6 +303,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,7 +619,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
+      <selection pane="bottomRight" activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1078,9 @@
       <c r="U8">
         <v>5</v>
       </c>
-      <c r="V8" s="9"/>
+      <c r="V8" s="14">
+        <v>5</v>
+      </c>
       <c r="W8">
         <v>5</v>
       </c>
@@ -1242,7 +1248,9 @@
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
-      <c r="V12" s="9"/>
+      <c r="V12" s="9">
+        <v>5</v>
+      </c>
       <c r="W12">
         <v>5</v>
       </c>
@@ -1322,7 +1330,9 @@
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
-      <c r="V14" s="9"/>
+      <c r="V14" s="9">
+        <v>5</v>
+      </c>
       <c r="W14">
         <v>5</v>
       </c>
@@ -1375,7 +1385,9 @@
       <c r="U15">
         <v>5</v>
       </c>
-      <c r="V15" s="9"/>
+      <c r="V15" s="15">
+        <v>5</v>
+      </c>
       <c r="W15">
         <v>5</v>
       </c>
@@ -1769,7 +1781,9 @@
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
-      <c r="V23" s="9"/>
+      <c r="V23" s="14">
+        <v>5</v>
+      </c>
       <c r="W23">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 21:23:43_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -619,7 +619,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V9" sqref="V9"/>
+      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -873,7 +873,9 @@
       <c r="S4" s="3">
         <v>5</v>
       </c>
-      <c r="T4" s="2"/>
+      <c r="T4" s="2">
+        <v>5</v>
+      </c>
       <c r="U4" s="11">
         <v>5</v>
       </c>
@@ -1187,6 +1189,9 @@
       <c r="Y10">
         <v>5</v>
       </c>
+      <c r="Z10">
+        <v>5</v>
+      </c>
       <c r="AA10">
         <v>22</v>
       </c>
@@ -1260,6 +1265,9 @@
       <c r="Y12">
         <v>5</v>
       </c>
+      <c r="Z12">
+        <v>5</v>
+      </c>
       <c r="AA12">
         <v>2</v>
       </c>
@@ -1330,6 +1338,9 @@
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
+      <c r="U14">
+        <v>5</v>
+      </c>
       <c r="V14" s="9">
         <v>5</v>
       </c>
@@ -1780,7 +1791,12 @@
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
+      <c r="T23" s="2">
+        <v>5</v>
+      </c>
+      <c r="U23">
+        <v>5</v>
+      </c>
       <c r="V23" s="14">
         <v>5</v>
       </c>
@@ -1788,6 +1804,12 @@
         <v>5</v>
       </c>
       <c r="X23">
+        <v>5</v>
+      </c>
+      <c r="Y23">
+        <v>5</v>
+      </c>
+      <c r="Z23">
         <v>5</v>
       </c>
       <c r="AA23">

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 21:27:32_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -619,7 +619,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -779,7 +779,9 @@
       </c>
       <c r="D3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="Q3" s="2">
+        <v>5</v>
+      </c>
       <c r="R3" s="2">
         <v>5</v>
       </c>
@@ -1787,10 +1789,14 @@
         <v>5</v>
       </c>
       <c r="Q23" s="3">
-        <v>4</v>
-      </c>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="R23" s="2">
+        <v>5</v>
+      </c>
+      <c r="S23" s="2">
+        <v>5</v>
+      </c>
       <c r="T23" s="2">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 8:14:45_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_ОпСис_.xlsx
@@ -619,7 +619,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1574,6 +1574,9 @@
       <c r="N19">
         <v>5</v>
       </c>
+      <c r="O19">
+        <v>5</v>
+      </c>
       <c r="P19" s="3">
         <v>5</v>
       </c>
@@ -1595,6 +1598,12 @@
         <v>5</v>
       </c>
       <c r="X19">
+        <v>5</v>
+      </c>
+      <c r="Y19">
+        <v>5</v>
+      </c>
+      <c r="Z19">
         <v>5</v>
       </c>
       <c r="AA19">

</xml_diff>